<commit_message>
delete fund_low,add batch operations on paper,improve xlsx download and set id-value hashmaps to be used
</commit_message>
<xml_diff>
--- a/standard/表格结构.xlsx
+++ b/standard/表格结构.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E766D128-16E3-4828-BE23-3B7BADBC86F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113F6039-2BE2-4554-901A-A1C73165AB61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,10 +136,6 @@
   </si>
   <si>
     <t>varchar(100)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>经费预算下界</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -562,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -574,18 +570,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -612,81 +596,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -971,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -991,13 +981,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -1018,18 +1008,18 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="25.5" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1047,12 +1037,12 @@
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1070,38 +1060,38 @@
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:10" ht="25.5" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
+      <c r="A9" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1123,139 +1113,139 @@
         <v>24</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10" s="48" t="s">
-        <v>79</v>
+        <v>37</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="49" t="s">
-        <v>84</v>
+      <c r="H11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="29" t="s">
+      <c r="A13" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="C14" s="4">
         <v>2</v>
       </c>
-      <c r="D14" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="D14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
+      <c r="A15" s="5">
         <v>0</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>43</v>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="4">
         <v>-2</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="10"/>
+      <c r="D15" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="14" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="A16" s="5">
         <v>1</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>-1</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-    </row>
-    <row r="17" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11">
-        <v>-1</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:14" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="1:14" ht="25.5" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="30"/>
+      <c r="A20" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="5"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1277,29 +1267,27 @@
         <v>31</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="M21" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="26" t="s">
-        <v>63</v>
-      </c>
+      <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1309,7 +1297,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>29</v>
@@ -1318,10 +1306,10 @@
         <v>8</v>
       </c>
       <c r="G22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>8</v>
@@ -1329,177 +1317,175 @@
       <c r="J22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L22" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="M22" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="N22" s="26" t="s">
-        <v>64</v>
-      </c>
+      <c r="K22" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="42"/>
+      <c r="A23" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="14"/>
     </row>
     <row r="24" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="23"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="14"/>
     </row>
     <row r="25" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:14" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="46" t="s">
+      <c r="A26" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="41"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="41"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="17" t="s">
+      <c r="E27" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>2</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="14">
+        <v>2</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="15">
+        <v>3</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="14">
+        <v>3</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="14">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D32" s="14">
+        <v>5</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="18">
+        <v>6</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <v>1</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="18">
-        <v>1</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="18">
-        <v>2</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="18">
-        <v>2</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19">
-        <v>3</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="18">
-        <v>3</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="18">
-        <v>4</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D32" s="18">
-        <v>5</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D33" s="25">
-        <v>6</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="34" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="44"/>
+      <c r="D34" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="26"/>
     </row>
     <row r="35" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D35" s="27"/>
@@ -1507,60 +1493,59 @@
     </row>
     <row r="36" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="37" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
+      <c r="A37" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="41"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="10" t="s">
+      <c r="B39" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="12" t="s">
+      <c r="D39" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="D34:E35"/>
-    <mergeCell ref="A23:N24"/>
     <mergeCell ref="C16:E17"/>
     <mergeCell ref="A37:F37"/>
     <mergeCell ref="A1:G1"/>
@@ -1571,6 +1556,7 @@
     <mergeCell ref="A20:K20"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A23:M24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>